<commit_message>
Update of DBTL0.1 data
</commit_message>
<xml_diff>
--- a/data/flaviolin/DBTL0.1/edd_OD340.xlsx
+++ b/data/flaviolin/DBTL0.1/edd_OD340.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -492,7 +492,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -515,7 +515,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -538,7 +538,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -561,7 +561,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -584,7 +584,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -676,7 +676,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -699,7 +699,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -722,7 +722,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -745,7 +745,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -768,7 +768,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -791,7 +791,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -814,7 +814,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -837,7 +837,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -860,7 +860,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -883,7 +883,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -929,7 +929,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -952,7 +952,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -975,7 +975,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -998,7 +998,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C49" t="n">

</xml_diff>

<commit_message>
DBTL 0.1 protocol files
</commit_message>
<xml_diff>
--- a/data/flaviolin/DBTL0.1/edd_OD340.xlsx
+++ b/data/flaviolin/DBTL0.1/edd_OD340.xlsx
@@ -469,7 +469,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -492,7 +492,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -515,7 +515,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -538,7 +538,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -561,7 +561,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -584,7 +584,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -607,7 +607,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -630,7 +630,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -676,7 +676,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -699,7 +699,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -722,7 +722,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -745,7 +745,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -768,7 +768,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -791,7 +791,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -814,7 +814,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -837,7 +837,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -860,7 +860,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -883,7 +883,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -906,7 +906,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -929,7 +929,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -952,7 +952,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -975,7 +975,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -998,7 +998,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1044,7 +1044,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1067,7 +1067,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1090,7 +1090,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1113,7 +1113,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1159,7 +1159,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1182,7 +1182,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1205,7 +1205,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1320,7 +1320,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1435,7 +1435,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1504,7 +1504,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1527,7 +1527,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>OD340</t>
+          <t>Optical Density</t>
         </is>
       </c>
       <c r="C49" t="n">

</xml_diff>